<commit_message>
2/3/17 Capture of sources. Have since moved to DD repo for farther work capturing other files as well.
</commit_message>
<xml_diff>
--- a/JsDev/DD_POC_v2/WorkRequest_WorkFlows-End-to-End_Tests.xlsx
+++ b/JsDev/DD_POC_v2/WorkRequest_WorkFlows-End-to-End_Tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="16815" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="16815" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Senior" sheetId="1" r:id="rId1"/>
@@ -722,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
@@ -1506,12 +1506,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C14:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>72</v>
+      </c>
+      <c r="F14">
+        <v>0.75</v>
+      </c>
+      <c r="G14">
+        <f>PRODUCT(C14:F14)</f>
+        <v>3888</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>